<commit_message>
Pressure sensor parameters calculated
</commit_message>
<xml_diff>
--- a/Schedules.xlsx
+++ b/Schedules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Androvil\Visual Studio 2013\Projects\HomeAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A543F0-C2E8-42D6-90FD-C8638197D633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253A8E44-9BC0-48F6-A0FB-57BA3FEB95F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15075" activeTab="3" xr2:uid="{BC55A6CB-6D2E-44AC-924D-E6CB2B85EFF9}"/>
+    <workbookView xWindow="-28920" yWindow="-480" windowWidth="29040" windowHeight="15525" activeTab="3" xr2:uid="{BC55A6CB-6D2E-44AC-924D-E6CB2B85EFF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Timer schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="1115">
   <si>
     <t>Mon, Aug 1</t>
   </si>
@@ -3348,6 +3348,39 @@
   </si>
   <si>
     <t>80 psi</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>calc(y)</t>
+  </si>
+  <si>
+    <t>calc(a)</t>
+  </si>
+  <si>
+    <t>avg(a)</t>
+  </si>
+  <si>
+    <t>y = a x + b</t>
+  </si>
+  <si>
+    <t>150 - 2</t>
+  </si>
+  <si>
+    <t>150 - 3</t>
+  </si>
+  <si>
+    <t>x (bar)</t>
+  </si>
+  <si>
+    <t>y (V)</t>
+  </si>
+  <si>
+    <t>x = (y - b) / a</t>
   </si>
 </sst>
 </file>
@@ -3463,10 +3496,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3860,6 +3893,12 @@
                 <c:pt idx="3">
                   <c:v>1.74</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.52</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3867,6 +3906,150 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-912B-45CF-B70E-6A7E684BE299}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Presure Sensors'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>150 - 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Presure Sensors'!$F$4:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5DE4-43A9-B6C3-D0EC7D7BEC36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Presure Sensors'!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>150 - 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Presure Sensors'!$G$4:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5DE4-43A9-B6C3-D0EC7D7BEC36}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4986,38 +5169,38 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="36">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37">
         <v>2</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36">
+      <c r="D2" s="37"/>
+      <c r="E2" s="37">
         <v>3</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36">
+      <c r="F2" s="37"/>
+      <c r="G2" s="37">
         <v>4</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36">
+      <c r="H2" s="37"/>
+      <c r="I2" s="37">
         <v>1</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36">
+      <c r="J2" s="37"/>
+      <c r="K2" s="37">
         <v>2</v>
       </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36">
+      <c r="L2" s="37"/>
+      <c r="M2" s="37">
         <v>3</v>
       </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36">
+      <c r="N2" s="37"/>
+      <c r="O2" s="37">
         <v>4</v>
       </c>
-      <c r="P2" s="36"/>
+      <c r="P2" s="37"/>
     </row>
     <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -5202,14 +5385,14 @@
       <c r="H1" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36" t="s">
+      <c r="J1" s="37"/>
+      <c r="K1" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="L1" s="36"/>
+      <c r="L1" s="37"/>
       <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -31212,15 +31395,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741B0702-5186-4FC0-8C5C-47996DD97BFF}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1103</v>
       </c>
@@ -31234,24 +31417,30 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1099</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>1098</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>1097</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="36" t="s">
         <v>1096</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="36" t="s">
         <v>1095</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="36" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -31267,8 +31456,14 @@
       <c r="E4">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0.54</v>
+      </c>
+      <c r="G4">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -31284,8 +31479,14 @@
       <c r="E5">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0.95</v>
+      </c>
+      <c r="G5">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -31301,8 +31502,14 @@
       <c r="E6">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1.34</v>
+      </c>
+      <c r="G6">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -31318,8 +31525,14 @@
       <c r="E7">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1.72</v>
+      </c>
+      <c r="G7">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -31332,8 +31545,17 @@
       <c r="D8">
         <v>3.43</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>2.11</v>
+      </c>
+      <c r="F8">
+        <v>2.11</v>
+      </c>
+      <c r="G8">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -31346,9 +31568,403 @@
       <c r="D9">
         <v>4.2</v>
       </c>
+      <c r="E9">
+        <v>2.52</v>
+      </c>
+      <c r="F9">
+        <v>2.48</v>
+      </c>
+      <c r="G9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B14">
+        <f>(B5-B$4)/$A5</f>
+        <v>0.81</v>
+      </c>
+      <c r="C14">
+        <f>(C5-C$4)/$A5</f>
+        <v>0.79</v>
+      </c>
+      <c r="D14">
+        <f>(D5-D$4)/$A5</f>
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="E14">
+        <f>(E5-E$4)/$A5</f>
+        <v>0.41999999999999993</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:G14" si="0">(F5-F$4)/$A5</f>
+        <v>0.40999999999999992</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:B18" si="1">(B6-B$4)/A6</f>
+        <v>0.76</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:G18" si="2">(C6-C$4)/$A6</f>
+        <v>0.745</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0.40500000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>0.75666666666666671</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0.7466666666666667</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0.39333333333333331</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>0.39999999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>0.75250000000000006</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:G17" si="3">(E8-E$4)/$A8</f>
+        <v>0.39249999999999996</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>0.39249999999999996</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>0.39249999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>0.74</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:G18" si="4">(E9-E$4)/$A9</f>
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B19">
+        <f>AVERAGE(B14:B18)</f>
+        <v>0.75946666666666673</v>
+      </c>
+      <c r="C19" s="8">
+        <f t="shared" ref="C19:G19" si="5">AVERAGE(C14:C18)</f>
+        <v>0.75683333333333336</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="5"/>
+        <v>0.76963333333333339</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="5"/>
+        <v>0.40169999999999995</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>0.3967666666666666</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>0.39789999999999992</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B21">
+        <f>B$4+$A4*B$19</f>
+        <v>0.48</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:G21" si="6">C$4+$A4*C$19</f>
+        <v>0.48</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="6"/>
+        <v>0.48</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="6"/>
+        <v>0.54</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="6"/>
+        <v>0.54</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="6"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:G26" si="7">B$4+$A5*B$19</f>
+        <v>1.2394666666666667</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="7"/>
+        <v>1.2368333333333332</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="7"/>
+        <v>1.2496333333333334</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="7"/>
+        <v>0.94169999999999998</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="7"/>
+        <v>0.93676666666666664</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="7"/>
+        <v>0.93789999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="7"/>
+        <v>1.9989333333333335</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="7"/>
+        <v>1.9936666666666667</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="7"/>
+        <v>2.0192666666666668</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="7"/>
+        <v>1.3433999999999999</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="7"/>
+        <v>1.3335333333333332</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>1.3357999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="7"/>
+        <v>2.7584000000000004</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="7"/>
+        <v>2.7505000000000002</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="7"/>
+        <v>2.7889000000000004</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>1.7450999999999999</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="7"/>
+        <v>1.7302999999999997</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="7"/>
+        <v>1.7336999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="7"/>
+        <v>3.5178666666666669</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="7"/>
+        <v>3.5073333333333334</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="7"/>
+        <v>3.5585333333333335</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="7"/>
+        <v>2.1467999999999998</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="7"/>
+        <v>2.1270666666666664</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="7"/>
+        <v>2.1315999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="7"/>
+        <v>4.277333333333333</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="7"/>
+        <v>4.2641666666666662</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="7"/>
+        <v>4.3281666666666663</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="7"/>
+        <v>2.5484999999999998</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="7"/>
+        <v>2.5238333333333332</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="7"/>
+        <v>2.5294999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B30">
+        <v>0.75683333333333336</v>
+      </c>
+      <c r="E30">
+        <v>0.3967666666666666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B31">
+        <v>0.48</v>
+      </c>
+      <c r="E31">
+        <v>0.54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>